<commit_message>
Update Please update this one tomorrow.xlsx
</commit_message>
<xml_diff>
--- a/db/Please update this one tomorrow.xlsx
+++ b/db/Please update this one tomorrow.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bizcom\Desktop\Javafx-AWS-RDS\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445EE024-902F-41C2-B4F4-040FE5071951}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C24C2-6061-4B25-BB91-26EC13F7076C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4800" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{CE4F9082-8BB9-4493-B760-4C14D8339CAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{CE4F9082-8BB9-4493-B760-4C14D8339CAE}"/>
   </bookViews>
   <sheets>
     <sheet name="p04 r17 firmware no assem" sheetId="1" r:id="rId1"/>
     <sheet name="p04 updated firmware no burnin" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="6" r:id="rId3"/>
+    <sheet name="112019" sheetId="6" r:id="rId3"/>
     <sheet name="assem upload firmware" sheetId="3" r:id="rId4"/>
     <sheet name="new fail" sheetId="5" r:id="rId5"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="179">
   <si>
     <t>stt</t>
   </si>
@@ -343,6 +343,237 @@
   </si>
   <si>
     <t>30N004000049</t>
+  </si>
+  <si>
+    <t>packed</t>
+  </si>
+  <si>
+    <t>30N004000391</t>
+  </si>
+  <si>
+    <t>30N004000401</t>
+  </si>
+  <si>
+    <t>30N004000066</t>
+  </si>
+  <si>
+    <t>30N004000228</t>
+  </si>
+  <si>
+    <t>30N004000105</t>
+  </si>
+  <si>
+    <t>30N004000195</t>
+  </si>
+  <si>
+    <t>30N004000002</t>
+  </si>
+  <si>
+    <t>30N004000152</t>
+  </si>
+  <si>
+    <t>30N004000162</t>
+  </si>
+  <si>
+    <t>30N004000227</t>
+  </si>
+  <si>
+    <t>SMC-P04 R17</t>
+  </si>
+  <si>
+    <t>30n004000196</t>
+  </si>
+  <si>
+    <t>30N004000283</t>
+  </si>
+  <si>
+    <t>30N004000116</t>
+  </si>
+  <si>
+    <t>30N004000377</t>
+  </si>
+  <si>
+    <t>30N004000239</t>
+  </si>
+  <si>
+    <t>30N004000058</t>
+  </si>
+  <si>
+    <t>30N004000200</t>
+  </si>
+  <si>
+    <t>30N004000325</t>
+  </si>
+  <si>
+    <t>30N004000188</t>
+  </si>
+  <si>
+    <t>30N004000314</t>
+  </si>
+  <si>
+    <t>30N004000234</t>
+  </si>
+  <si>
+    <t>30N004000334</t>
+  </si>
+  <si>
+    <t>30N004000106</t>
+  </si>
+  <si>
+    <t>30N004000372</t>
+  </si>
+  <si>
+    <t>30N004000068</t>
+  </si>
+  <si>
+    <t>30N004000375</t>
+  </si>
+  <si>
+    <t>30N004000103</t>
+  </si>
+  <si>
+    <t>30N004000226</t>
+  </si>
+  <si>
+    <t>30N004000368</t>
+  </si>
+  <si>
+    <t>30N004000323</t>
+  </si>
+  <si>
+    <t>30N004000346</t>
+  </si>
+  <si>
+    <t>30N004000373</t>
+  </si>
+  <si>
+    <t>30N004000110</t>
+  </si>
+  <si>
+    <t>30N004000376</t>
+  </si>
+  <si>
+    <t>30N004000121</t>
+  </si>
+  <si>
+    <t>30n004000230</t>
+  </si>
+  <si>
+    <t>30n004000093</t>
+  </si>
+  <si>
+    <t>30n004000081</t>
+  </si>
+  <si>
+    <t>30n004000313</t>
+  </si>
+  <si>
+    <t>30n004000213</t>
+  </si>
+  <si>
+    <t>30n004000367</t>
+  </si>
+  <si>
+    <t>30n004000395</t>
+  </si>
+  <si>
+    <t>30n004000143</t>
+  </si>
+  <si>
+    <t>30n004000198</t>
+  </si>
+  <si>
+    <t>30n004000020</t>
+  </si>
+  <si>
+    <t>30n004000091</t>
+  </si>
+  <si>
+    <t>30n004000189</t>
+  </si>
+  <si>
+    <t>30n004000101</t>
+  </si>
+  <si>
+    <t>30n004000139</t>
+  </si>
+  <si>
+    <t>30n004000140</t>
+  </si>
+  <si>
+    <t>30n004000206</t>
+  </si>
+  <si>
+    <t>30n004000128</t>
+  </si>
+  <si>
+    <t>30n004000374</t>
+  </si>
+  <si>
+    <t>30n004000306</t>
+  </si>
+  <si>
+    <t>30n004000013</t>
+  </si>
+  <si>
+    <t>30N004000007</t>
+  </si>
+  <si>
+    <t>30N004000378</t>
+  </si>
+  <si>
+    <t>30N004000238</t>
+  </si>
+  <si>
+    <t>30N004000022</t>
+  </si>
+  <si>
+    <t>30N004000399</t>
+  </si>
+  <si>
+    <t>30N004000333</t>
+  </si>
+  <si>
+    <t>30N004000211</t>
+  </si>
+  <si>
+    <t>30N004000324</t>
+  </si>
+  <si>
+    <t>30N004000369</t>
+  </si>
+  <si>
+    <t>30N004000347</t>
+  </si>
+  <si>
+    <t>30N004000141</t>
+  </si>
+  <si>
+    <t>30N004000402</t>
+  </si>
+  <si>
+    <t>30N004000039</t>
+  </si>
+  <si>
+    <t>30N004000118</t>
+  </si>
+  <si>
+    <t>30N004000194</t>
+  </si>
+  <si>
+    <t>30N004000319</t>
+  </si>
+  <si>
+    <t>30N004000019</t>
+  </si>
+  <si>
+    <t>30N004000109</t>
+  </si>
+  <si>
+    <t>30N004000229</t>
+  </si>
+  <si>
+    <t>30N004000335</t>
   </si>
 </sst>
 </file>
@@ -704,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E415887-81C8-46B5-8F10-37A97DBE9218}">
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,7 +2172,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,15 +2267,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288860F8-B1F9-4E34-8D7B-A7E71183E4F1}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96:D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2207,39 +2439,648 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>106</v>
+      </c>
+      <c r="D43" t="s">
+        <v>102</v>
+      </c>
+      <c r="I43" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>120</v>
+      </c>
+      <c r="D58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" t="s">
+        <v>102</v>
+      </c>
+      <c r="J59" t="s">
+        <v>10</v>
+      </c>
+      <c r="M59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="D64" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>127</v>
+      </c>
+      <c r="D65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>128</v>
+      </c>
+      <c r="D66" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>129</v>
+      </c>
+      <c r="D67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>131</v>
+      </c>
+      <c r="D69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>132</v>
+      </c>
+      <c r="D70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>134</v>
+      </c>
+      <c r="D72" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>135</v>
+      </c>
+      <c r="D73" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>136</v>
+      </c>
+      <c r="D74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>137</v>
+      </c>
+      <c r="D75" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>138</v>
+      </c>
+      <c r="D76" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>139</v>
+      </c>
+      <c r="D77" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>140</v>
+      </c>
+      <c r="D78" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>141</v>
+      </c>
+      <c r="D79" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>142</v>
+      </c>
+      <c r="D80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>143</v>
+      </c>
+      <c r="D81" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>144</v>
+      </c>
+      <c r="D82" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>145</v>
+      </c>
+      <c r="D83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>146</v>
+      </c>
+      <c r="D84" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>147</v>
+      </c>
+      <c r="D85" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>148</v>
+      </c>
+      <c r="D86" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>149</v>
+      </c>
+      <c r="D87" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>150</v>
+      </c>
+      <c r="D88" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>151</v>
+      </c>
+      <c r="D89" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>152</v>
+      </c>
+      <c r="D90" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>153</v>
+      </c>
+      <c r="D91" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>154</v>
+      </c>
+      <c r="D92" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>155</v>
+      </c>
+      <c r="D93" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>156</v>
+      </c>
+      <c r="D94" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>157</v>
+      </c>
+      <c r="D95" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>158</v>
+      </c>
+      <c r="D96" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>159</v>
+      </c>
+      <c r="D97" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>160</v>
+      </c>
+      <c r="D98" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>161</v>
+      </c>
+      <c r="D99" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>162</v>
+      </c>
+      <c r="D100" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>163</v>
+      </c>
+      <c r="D101" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>164</v>
+      </c>
+      <c r="D102" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>165</v>
+      </c>
+      <c r="D103" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>166</v>
+      </c>
+      <c r="D104" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>167</v>
+      </c>
+      <c r="D105" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>168</v>
+      </c>
+      <c r="D106" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>169</v>
+      </c>
+      <c r="D107" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>170</v>
+      </c>
+      <c r="D108" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>171</v>
+      </c>
+      <c r="D109" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>172</v>
+      </c>
+      <c r="D110" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>173</v>
+      </c>
+      <c r="D111" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>174</v>
+      </c>
+      <c r="D112" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>175</v>
+      </c>
+      <c r="D113" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>176</v>
+      </c>
+      <c r="D114" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>177</v>
+      </c>
+      <c r="D115" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>178</v>
+      </c>
+      <c r="D116" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>